<commit_message>
Updates and adds files from Lab
</commit_message>
<xml_diff>
--- a/secData2.xlsx
+++ b/secData2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\PycharmProjects\python-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C2FAED-744F-452E-9C59-72B1CEF79EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4E363-3CA3-421A-8EB5-5642DE43B79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1725" windowWidth="21600" windowHeight="13620" activeTab="1" xr2:uid="{D481F55A-4EF9-4804-9C01-9BC1232C6DB2}"/>
+    <workbookView xWindow="2640" yWindow="1725" windowWidth="21600" windowHeight="13620" xr2:uid="{D481F55A-4EF9-4804-9C01-9BC1232C6DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF68B899-B517-4C06-B6AA-6DDDB06CF28F}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="9">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -714,7 +714,7 @@
       </c>
       <c r="Q3" s="9">
         <f>I3*0.6</f>
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
@@ -739,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="9">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="Q4" s="9">
         <f t="shared" ref="Q4:Q8" si="0">I4*0.6</f>
-        <v>6.0000000000000001E-3</v>
+        <v>0.06</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
@@ -773,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="9">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -784,7 +784,7 @@
       </c>
       <c r="Q5" s="9">
         <f t="shared" si="0"/>
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
@@ -807,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="9">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="Q6" s="9">
         <f t="shared" si="0"/>
-        <v>0.54</v>
+        <v>0.12</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="9">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -846,7 +846,7 @@
       </c>
       <c r="Q7" s="9">
         <f>I7*0.6</f>
-        <v>6.0000000000000001E-3</v>
+        <v>0.06</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
@@ -862,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="16">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
@@ -873,7 +873,7 @@
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="0"/>
-        <v>6.0000000000000001E-3</v>
+        <v>0.06</v>
       </c>
       <c r="R8" s="16"/>
       <c r="S8" s="16"/>
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="5">
         <v>5</v>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A83701-554A-49EA-BEFF-31A40D4F0692}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3958,7 +3958,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4998,21 +4998,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA6FEDBE726A3D4BB6A3DD1FC423C645" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5b46a3744ab63b46ac8390338c0ec29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1685e70-4409-44ff-a129-d9557ed9b25b" xmlns:ns4="dd78913b-84cb-4e23-9d1e-766268695023" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="101e21a860029da8357ea7a2996377f6" ns3:_="" ns4:_="">
     <xsd:import namespace="e1685e70-4409-44ff-a129-d9557ed9b25b"/>
@@ -5223,32 +5208,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F22E367B-3987-45E2-9C94-F1D93CDCEDA6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e1685e70-4409-44ff-a129-d9557ed9b25b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dd78913b-84cb-4e23-9d1e-766268695023"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC684770-FBB1-48C7-813E-0130852B6127}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5295C7A2-8A6E-4C6B-A9EC-7FF17D31CF74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5265,4 +5240,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC684770-FBB1-48C7-813E-0130852B6127}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F22E367B-3987-45E2-9C94-F1D93CDCEDA6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e1685e70-4409-44ff-a129-d9557ed9b25b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dd78913b-84cb-4e23-9d1e-766268695023"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>